<commit_message>
hola juan tooday in the afternoon change the button with power bi model
</commit_message>
<xml_diff>
--- a/pwbi/Modello Strutturale/Excell Power bi strutt.xlsx
+++ b/pwbi/Modello Strutturale/Excell Power bi strutt.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\TESI\website\Web-Thesis\pwbi\Modello Strutturale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DB3840-4821-41C2-A5A0-E221FF089446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2100928-D2D3-409F-AC28-D794DF4DB275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E29DDDD-077D-40F2-89EF-4627DB13E924}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3E29DDDD-077D-40F2-89EF-4627DB13E924}"/>
   </bookViews>
   <sheets>
     <sheet name="finaltable strutt" sheetId="2" r:id="rId1"/>
+    <sheet name="Momento Flettente" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="44">
   <si>
     <t>ID Beam</t>
   </si>
@@ -166,6 +167,9 @@
   <si>
     <t>P012</t>
   </si>
+  <si>
+    <t>Mtot (KNm)</t>
+  </si>
 </sst>
 </file>
 
@@ -200,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,8 +217,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -391,13 +407,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -441,9 +486,18 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Colore 1 2" xfId="1" xr:uid="{89051A78-0149-4E74-A55B-3193F5DEF281}"/>
+    <cellStyle name="20% - Colore 5" xfId="3" builtinId="46"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 2" xfId="2" xr:uid="{2B1F7243-1E3A-4CFB-B347-CBA156CA511B}"/>
   </cellStyles>
@@ -759,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1268B89D-5F78-4DBE-A04E-3C370254AEF6}">
   <dimension ref="A1:F265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
-      <selection activeCell="E261" sqref="E261"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4753,4 +4807,2939 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB5CB67-1A95-48B5-B568-19672EB5D506}">
+  <dimension ref="A1:C265"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134:C145"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="16">
+        <v>-24.767700000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="17">
+        <v>-2758.7687999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="17">
+        <v>-4990.9177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="17">
+        <v>-6100.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="17">
+        <v>-7092.7624999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="17">
+        <v>-7805.0649999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="17">
+        <v>-7804.0931</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="17">
+        <v>-7097.1291000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="17">
+        <v>-6138.8477000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="17">
+        <v>-4998.7523000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="17">
+        <v>-2822.1734999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="17">
+        <v>-30.532399999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="17">
+        <v>-37.709400000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="17">
+        <v>-2786.0252999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="17">
+        <v>-4998.0618000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="17">
+        <v>-6290.7083000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="17">
+        <v>-6948.4461000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="17">
+        <v>-7487.6127999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="17">
+        <v>-7487.6190999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="17">
+        <v>-6988.5023000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="17">
+        <v>-6297.3018000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="17">
+        <v>-5004.3755000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="17">
+        <v>-2864.8074000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="17">
+        <v>-43.296399999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="17">
+        <f>-43.8158</f>
+        <v>-43.815800000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="17">
+        <v>-2789.7573000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="17">
+        <v>-4806.2042000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="17">
+        <v>-6064.1633000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="17">
+        <v>-6836.3109999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="17">
+        <v>-7428.6032999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="17">
+        <v>-7428.5562</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="17">
+        <v>-6875.8712999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="17">
+        <v>-6099.1364000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="17">
+        <v>-4800.9036999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="17">
+        <v>-2875.1511</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="17">
+        <v>-48.905200000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="17">
+        <v>-45.0869</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="17">
+        <v>-2787.0722000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="17">
+        <v>-5005.6668</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="17">
+        <v>-5995.1804000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="17">
+        <v>-6821.9110000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="17">
+        <v>-7408.7363999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="17">
+        <v>-7408.6424999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="17">
+        <v>-6861.5077000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="17">
+        <v>-5998.6752999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="17">
+        <v>-5008.9477999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="17">
+        <v>-2873.9838</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="17">
+        <v>-50.113599999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" s="17">
+        <v>-45.3127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="17">
+        <v>-2783.2550999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" s="17">
+        <v>-4997.2620999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="17">
+        <v>-5987.1971000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54" s="17">
+        <v>-6812.1867000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" s="17">
+        <v>-7399.6531000000004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C56" s="17">
+        <v>-7399.5343999999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="17">
+        <v>-6852.2812999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" s="17">
+        <v>-5989.5061999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" s="17">
+        <v>-4999.4296999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="17">
+        <v>-2869.8816000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="17">
+        <v>-50.433300000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62" s="17">
+        <v>-45.375900000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="17">
+        <v>-2779.4349000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" s="17">
+        <v>-4988.6936999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" s="17">
+        <v>-5948.5532000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" s="17">
+        <v>-6803.5303999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" s="17">
+        <v>-7392.8975</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C68" s="17">
+        <v>-7392.7833000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C69" s="17">
+        <v>-6843.8477000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C70" s="17">
+        <v>-5949.6054999999997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C71" s="17">
+        <v>-4989.6923999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C72" s="17">
+        <v>-2864.951</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C73" s="17">
+        <v>-50.422899999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C74" s="17">
+        <v>-45.849699999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" s="17">
+        <v>-2779.2777999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76" s="17">
+        <v>-4985.3296</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C77" s="17">
+        <v>-5944.2277999999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C78" s="17">
+        <v>-6894.0428000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C79" s="17">
+        <v>-7378.9543000000003</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C80" s="17">
+        <v>-7378.8783000000003</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C81" s="17">
+        <v>-6833.2356</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C82" s="17">
+        <v>-5943.3131000000003</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83" s="17">
+        <v>-4984.5164000000004</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C84" s="17">
+        <v>-2862.6385</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85" s="17">
+        <v>-50.271700000000003</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C86" s="17">
+        <v>-46.784700000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C87" s="17">
+        <v>-2788.6621</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C88" s="17">
+        <v>-4997.0469999999996</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C89" s="17">
+        <v>-5952.5698000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C90" s="17">
+        <v>-6780.9539000000004</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C91" s="17">
+        <v>-7344.7932000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C92" s="17">
+        <v>-7344.8094000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" s="17">
+        <v>-6815.7107999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C94" s="17">
+        <v>-6048.6269000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C95" s="17">
+        <v>-4993.4609</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C96" s="17">
+        <v>-2867.4038999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C97" s="17">
+        <v>-49.205199999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C98" s="17">
+        <v>-47.141300000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C99" s="17">
+        <v>-2819.4769000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C100" s="17">
+        <v>-5035.3653000000004</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C101" s="17">
+        <v>-5982.0754999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C102" s="17">
+        <v>-6860.5173000000004</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C103" s="17">
+        <v>-7276.7165999999997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C104" s="17">
+        <v>-7276.9254000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C105" s="17">
+        <v>-6885.3500999999997</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C106" s="17">
+        <v>-5974.8158999999996</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C107" s="17">
+        <v>-5028.8861999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C108" s="17">
+        <v>-2885.7818000000002</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C109" s="17">
+        <v>-44.346800000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C110" s="18">
+        <v>-43.677399999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C111" s="18">
+        <v>-2876.2361999999998</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C112" s="18">
+        <v>-5048.8477000000003</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C113" s="18">
+        <v>-5887.5897999999997</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C114" s="18">
+        <v>-6761.8710000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C115" s="18">
+        <v>-7164.2683999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C116" s="18">
+        <v>-7164.5889999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C117" s="18">
+        <v>-6775.5554000000002</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C118" s="18">
+        <v>-5878.1598999999997</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C119" s="18">
+        <v>-5040.3643000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C120" s="18">
+        <v>-2924.6305000000002</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C121" s="18">
+        <v>-35.134300000000003</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C122" s="18">
+        <v>-37.905700000000003</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C123" s="18">
+        <v>-2906.8301999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C124" s="18">
+        <v>-5046.1896999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C125" s="18">
+        <v>-5884.4795999999997</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C126" s="18">
+        <v>-6665.3921</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C127" s="18">
+        <v>-7057.8204999999998</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C128" s="18">
+        <v>-7058.1634999999997</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C129" s="18">
+        <v>-6682.3724000000002</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C130" s="18">
+        <v>-5874.0210999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C131" s="18">
+        <v>-5036.6459000000004</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C132" s="18">
+        <v>-2945.6817000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C133" s="18">
+        <v>-26.910299999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C134" s="18">
+        <v>-37.905700000000003</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C135" s="18">
+        <v>-2906.8301999999999</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C136" s="18">
+        <v>-5046.1896999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C137" s="18">
+        <v>-5884.4795999999997</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C138" s="18">
+        <v>-6665.3921</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C139" s="18">
+        <v>-7057.8204999999998</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C140" s="18">
+        <v>-7058.1634999999997</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C141" s="18">
+        <v>-6682.3724000000002</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C142" s="18">
+        <v>-5874.0210999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C143" s="18">
+        <v>-5036.6459000000004</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C144" s="18">
+        <v>-2945.6817000000001</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C145" s="18">
+        <v>-26.910299999999999</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C146" s="18">
+        <v>-43.677399999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C147" s="18">
+        <v>-2876.2361999999998</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C148" s="18">
+        <v>-5048.8477000000003</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C149" s="18">
+        <v>-5887.5897999999997</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C150" s="18">
+        <v>-6761.8710000000001</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C151" s="18">
+        <v>-7164.2683999999999</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C152" s="18">
+        <v>-7164.5889999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C153" s="18">
+        <v>-6775.5554000000002</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C154" s="18">
+        <v>-5878.1598999999997</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C155" s="18">
+        <v>-5040.3643000000002</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C156" s="18">
+        <v>-2924.6305000000002</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C157" s="18">
+        <v>-35.134300000000003</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C158" s="17">
+        <v>-47.141300000000001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B159" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C159" s="17">
+        <v>-2819.4769000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C160" s="17">
+        <v>-5035.3653000000004</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C161" s="17">
+        <v>-5982.0754999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C162" s="17">
+        <v>-6860.5173000000004</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C163" s="17">
+        <v>-7276.7165999999997</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C164" s="17">
+        <v>-7276.9254000000001</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C165" s="17">
+        <v>-6885.3500999999997</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B166" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C166" s="17">
+        <v>-5974.8158999999996</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C167" s="17">
+        <v>-5028.8861999999999</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C168" s="17">
+        <v>-2885.7818000000002</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B169" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C169" s="17">
+        <v>-44.346800000000002</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C170" s="17">
+        <v>-46.784700000000001</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B171" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C171" s="17">
+        <v>-2788.6621</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C172" s="17">
+        <v>-4997.0469999999996</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B173" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C173" s="17">
+        <v>-5952.5698000000002</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C174" s="17">
+        <v>-6780.9539000000004</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B175" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C175" s="17">
+        <v>-7344.7932000000001</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C176" s="17">
+        <v>-7344.8094000000001</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B177" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C177" s="17">
+        <v>-6815.7107999999998</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C178" s="17">
+        <v>-6048.6269000000002</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B179" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C179" s="17">
+        <v>-4993.4609</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C180" s="17">
+        <v>-2867.4038999999998</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A181" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C181" s="17">
+        <v>-49.205199999999998</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C182" s="17">
+        <v>-45.849699999999999</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C183" s="17">
+        <v>-2779.2777999999998</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C184" s="17">
+        <v>-4985.3296</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A185" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C185" s="17">
+        <v>-5944.2277999999997</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B186" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C186" s="17">
+        <v>-6894.0428000000002</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C187" s="17">
+        <v>-7378.9543000000003</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C188" s="17">
+        <v>-7378.8783000000003</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C189" s="17">
+        <v>-6833.2356</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C190" s="17">
+        <v>-5943.3131000000003</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B191" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C191" s="17">
+        <v>-4984.5164000000004</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C192" s="17">
+        <v>-2862.6385</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B193" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C193" s="17">
+        <v>-50.271700000000003</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C194" s="17">
+        <v>-45.375900000000001</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B195" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C195" s="17">
+        <v>-2779.4349000000002</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C196" s="17">
+        <v>-4988.6936999999998</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B197" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C197" s="17">
+        <v>-5948.5532000000003</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C198" s="17">
+        <v>-6803.5303999999996</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C199" s="17">
+        <v>-7392.8975</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C200" s="17">
+        <v>-7392.7833000000001</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B201" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C201" s="17">
+        <v>-6843.8477000000003</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B202" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C202" s="17">
+        <v>-5949.6054999999997</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A203" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B203" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C203" s="17">
+        <v>-4989.6923999999999</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A204" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C204" s="17">
+        <v>-2864.951</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A205" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B205" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C205" s="17">
+        <v>-50.422899999999998</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A206" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C206" s="17">
+        <v>-45.3127</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A207" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B207" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C207" s="17">
+        <v>-2783.2550999999999</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A208" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B208" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C208" s="17">
+        <v>-4997.2620999999999</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A209" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B209" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C209" s="17">
+        <v>-5987.1971000000003</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A210" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B210" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C210" s="17">
+        <v>-6812.1867000000002</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A211" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B211" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C211" s="17">
+        <v>-7399.6531000000004</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A212" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B212" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C212" s="17">
+        <v>-7399.5343999999996</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A213" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B213" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C213" s="17">
+        <v>-6852.2812999999996</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A214" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B214" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C214" s="17">
+        <v>-5989.5061999999998</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A215" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B215" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C215" s="17">
+        <v>-4999.4296999999997</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A216" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B216" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C216" s="17">
+        <v>-2869.8816000000002</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A217" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B217" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C217" s="17">
+        <v>-50.433300000000003</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A218" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B218" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C218" s="17">
+        <v>-45.0869</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A219" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B219" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C219" s="17">
+        <v>-2787.0722000000001</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A220" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B220" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C220" s="17">
+        <v>-5005.6668</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A221" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B221" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C221" s="17">
+        <v>-5995.1804000000002</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A222" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B222" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C222" s="17">
+        <v>-6821.9110000000001</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A223" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B223" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C223" s="17">
+        <v>-7408.7363999999998</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A224" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B224" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C224" s="17">
+        <v>-7408.6424999999999</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A225" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B225" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C225" s="17">
+        <v>-6861.5077000000001</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A226" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B226" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C226" s="17">
+        <v>-5998.6752999999999</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A227" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B227" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C227" s="17">
+        <v>-5008.9477999999999</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A228" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B228" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C228" s="17">
+        <v>-2873.9838</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A229" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B229" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C229" s="17">
+        <v>-50.113599999999998</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A230" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B230" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C230" s="17">
+        <f>-43.8158</f>
+        <v>-43.815800000000003</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A231" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B231" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C231" s="17">
+        <v>-2789.7573000000002</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A232" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B232" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C232" s="17">
+        <v>-4806.2042000000001</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A233" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B233" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C233" s="17">
+        <v>-6064.1633000000002</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A234" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B234" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C234" s="17">
+        <v>-6836.3109999999997</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A235" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B235" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C235" s="17">
+        <v>-7428.6032999999998</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A236" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C236" s="17">
+        <v>-7428.5562</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A237" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B237" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C237" s="17">
+        <v>-6875.8712999999998</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A238" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B238" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C238" s="17">
+        <v>-6099.1364000000003</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A239" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B239" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C239" s="17">
+        <v>-4800.9036999999998</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A240" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B240" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C240" s="17">
+        <v>-2875.1511</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A241" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B241" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C241" s="17">
+        <v>-48.905200000000001</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A242" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C242" s="17">
+        <v>-37.709400000000002</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A243" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B243" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C243" s="17">
+        <v>-2786.0252999999998</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A244" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B244" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C244" s="17">
+        <v>-4998.0618000000004</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A245" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B245" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C245" s="17">
+        <v>-6290.7083000000002</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A246" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B246" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C246" s="17">
+        <v>-6948.4461000000001</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A247" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B247" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C247" s="17">
+        <v>-7487.6127999999999</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A248" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C248" s="17">
+        <v>-7487.6190999999999</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A249" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B249" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C249" s="17">
+        <v>-6988.5023000000001</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A250" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B250" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C250" s="17">
+        <v>-6297.3018000000002</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A251" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B251" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C251" s="17">
+        <v>-5004.3755000000001</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A252" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C252" s="17">
+        <v>-2864.8074000000001</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A253" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B253" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C253" s="17">
+        <v>-43.296399999999998</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A254" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C254" s="16">
+        <v>-24.767700000000001</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A255" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B255" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C255" s="17">
+        <v>-2758.7687999999998</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A256" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B256" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C256" s="17">
+        <v>-4990.9177</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A257" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B257" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C257" s="17">
+        <v>-6100.8</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A258" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B258" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C258" s="17">
+        <v>-7092.7624999999998</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A259" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B259" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C259" s="17">
+        <v>-7805.0649999999996</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A260" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B260" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C260" s="17">
+        <v>-7804.0931</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A261" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B261" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C261" s="17">
+        <v>-7097.1291000000001</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A262" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B262" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C262" s="17">
+        <v>-6138.8477000000003</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A263" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B263" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C263" s="17">
+        <v>-4998.7523000000001</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A264" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B264" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C264" s="17">
+        <v>-2822.1734999999999</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A265" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B265" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C265" s="17">
+        <v>-30.532399999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>